<commit_message>
finished the lesson 4 on pandas
</commit_message>
<xml_diff>
--- a/data/lettuce.xlsx
+++ b/data/lettuce.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Freshweight" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="43">
   <si>
     <t xml:space="preserve">Treatment</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">all in (g)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sampleno</t>
   </si>
   <si>
     <t xml:space="preserve">Plants</t>
@@ -246,12 +243,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -261,18 +258,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -286,7 +284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -300,7 +298,7 @@
         <v>363.755</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -314,7 +312,7 @@
         <v>233.54</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
@@ -328,7 +326,7 @@
         <v>368.57</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>4</v>
       </c>
@@ -342,7 +340,7 @@
         <v>336.96</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>4</v>
       </c>
@@ -356,7 +354,7 @@
         <v>357.88</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>4</v>
       </c>
@@ -370,7 +368,7 @@
         <v>270.015</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>4</v>
       </c>
@@ -384,7 +382,7 @@
         <v>339.87</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>4</v>
       </c>
@@ -398,7 +396,7 @@
         <v>326.425</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>4</v>
       </c>
@@ -412,7 +410,7 @@
         <v>269.731</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>4</v>
       </c>
@@ -426,7 +424,7 @@
         <v>370.031</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>4</v>
       </c>
@@ -440,7 +438,7 @@
         <v>353.409</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>4</v>
       </c>
@@ -454,7 +452,7 @@
         <v>373.66</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>4</v>
       </c>
@@ -468,7 +466,7 @@
         <v>345.58</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>4</v>
       </c>
@@ -482,7 +480,7 @@
         <v>372.64</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>4</v>
       </c>
@@ -496,7 +494,7 @@
         <v>369.58</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>4</v>
       </c>
@@ -510,7 +508,7 @@
         <v>228.04</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>4</v>
       </c>
@@ -524,7 +522,7 @@
         <v>373.68</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>4</v>
       </c>
@@ -538,7 +536,7 @@
         <v>340.84</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>4</v>
       </c>
@@ -552,7 +550,7 @@
         <v>316.643</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>4</v>
       </c>
@@ -566,7 +564,7 @@
         <v>223.658</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>4</v>
       </c>
@@ -580,7 +578,7 @@
         <v>343.705</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>4</v>
       </c>
@@ -594,7 +592,7 @@
         <v>321.74</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>4</v>
       </c>
@@ -608,7 +606,7 @@
         <v>166.23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>4</v>
       </c>
@@ -622,7 +620,7 @@
         <v>332.145</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>4</v>
       </c>
@@ -636,7 +634,7 @@
         <v>326.7</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>4</v>
       </c>
@@ -650,7 +648,7 @@
         <v>354.67</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>4</v>
       </c>
@@ -664,7 +662,7 @@
         <v>332.31</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>4</v>
       </c>
@@ -678,7 +676,7 @@
         <v>345.76</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>4</v>
       </c>
@@ -692,7 +690,7 @@
         <v>353.235</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>4</v>
       </c>
@@ -706,7 +704,7 @@
         <v>365.88</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>4</v>
       </c>
@@ -720,7 +718,7 @@
         <v>381.705</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>4</v>
       </c>
@@ -734,7 +732,7 @@
         <v>361.001</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>4</v>
       </c>
@@ -748,7 +746,7 @@
         <v>386.21</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>4</v>
       </c>
@@ -762,7 +760,7 @@
         <v>378.16</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>4</v>
       </c>
@@ -776,7 +774,7 @@
         <v>263.784</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>4</v>
       </c>
@@ -790,7 +788,7 @@
         <v>360.56</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>4</v>
       </c>
@@ -804,7 +802,7 @@
         <v>365.34</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>4</v>
       </c>
@@ -818,7 +816,7 @@
         <v>335.38</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>4</v>
       </c>
@@ -832,7 +830,7 @@
         <v>364.829</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>4</v>
       </c>
@@ -846,7 +844,7 @@
         <v>304.678</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>4</v>
       </c>
@@ -860,7 +858,7 @@
         <v>368.76</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>4</v>
       </c>
@@ -874,7 +872,7 @@
         <v>308.38</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>4</v>
       </c>
@@ -888,7 +886,7 @@
         <v>349.45</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>4</v>
       </c>
@@ -902,7 +900,7 @@
         <v>409.19</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>4</v>
       </c>
@@ -916,7 +914,7 @@
         <v>412.09</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>4</v>
       </c>
@@ -930,7 +928,7 @@
         <v>318.878</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>4</v>
       </c>
@@ -944,7 +942,7 @@
         <v>410.6</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>4</v>
       </c>
@@ -958,7 +956,7 @@
         <v>404.008</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>4</v>
       </c>
@@ -972,7 +970,7 @@
         <v>366.55</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>4</v>
       </c>
@@ -986,7 +984,7 @@
         <v>406.45</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>4</v>
       </c>
@@ -999,12 +997,8 @@
       <c r="D52" s="0" t="n">
         <v>366.98</v>
       </c>
-      <c r="E52" s="0" t="n">
-        <f aca="false">AVERAGE(D2:D52)</f>
-        <v>341.173823529412</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +1012,7 @@
         <v>222.815</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1026,7 @@
         <v>350.83</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>5</v>
       </c>
@@ -1046,7 +1040,7 @@
         <v>351.27</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>5</v>
       </c>
@@ -1060,7 +1054,7 @@
         <v>192.246</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>5</v>
       </c>
@@ -1074,7 +1068,7 @@
         <v>330.07</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>5</v>
       </c>
@@ -1088,7 +1082,7 @@
         <v>289.04</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>5</v>
       </c>
@@ -1102,7 +1096,7 @@
         <v>296.79</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>5</v>
       </c>
@@ -1116,7 +1110,7 @@
         <v>322.505</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>5</v>
       </c>
@@ -1130,7 +1124,7 @@
         <v>354.665</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>5</v>
       </c>
@@ -1144,7 +1138,7 @@
         <v>338.465</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>5</v>
       </c>
@@ -1158,7 +1152,7 @@
         <v>395.56</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>5</v>
       </c>
@@ -1172,7 +1166,7 @@
         <v>377.185</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>5</v>
       </c>
@@ -1186,7 +1180,7 @@
         <v>357.285</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>5</v>
       </c>
@@ -1200,7 +1194,7 @@
         <v>358.97</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>5</v>
       </c>
@@ -1214,7 +1208,7 @@
         <v>310.1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1222,7 @@
         <v>364.985</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>5</v>
       </c>
@@ -1242,7 +1236,7 @@
         <v>374.57</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1250,7 @@
         <v>359.71</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>5</v>
       </c>
@@ -1270,7 +1264,7 @@
         <v>403.33</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>5</v>
       </c>
@@ -1284,7 +1278,7 @@
         <v>369.7</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>5</v>
       </c>
@@ -1298,7 +1292,7 @@
         <v>294.04</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>5</v>
       </c>
@@ -1312,7 +1306,7 @@
         <v>389.6</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>5</v>
       </c>
@@ -1326,7 +1320,7 @@
         <v>328.84</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>5</v>
       </c>
@@ -1340,7 +1334,7 @@
         <v>376.04</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>5</v>
       </c>
@@ -1354,7 +1348,7 @@
         <v>319.37</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>5</v>
       </c>
@@ -1368,7 +1362,7 @@
         <v>366.1</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>5</v>
       </c>
@@ -1382,7 +1376,7 @@
         <v>368.72</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>5</v>
       </c>
@@ -1396,7 +1390,7 @@
         <v>379.4</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>5</v>
       </c>
@@ -1410,7 +1404,7 @@
         <v>337.84</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>5</v>
       </c>
@@ -1424,7 +1418,7 @@
         <v>366.28</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>5</v>
       </c>
@@ -1438,7 +1432,7 @@
         <v>394.64</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>5</v>
       </c>
@@ -1452,7 +1446,7 @@
         <v>343.35</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>5</v>
       </c>
@@ -1466,7 +1460,7 @@
         <v>393.345</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>5</v>
       </c>
@@ -1480,7 +1474,7 @@
         <v>407.6</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>5</v>
       </c>
@@ -1494,7 +1488,7 @@
         <v>350.82</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>5</v>
       </c>
@@ -1508,7 +1502,7 @@
         <v>310.08</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>5</v>
       </c>
@@ -1522,7 +1516,7 @@
         <v>401.08</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>5</v>
       </c>
@@ -1536,7 +1530,7 @@
         <v>652.65</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>5</v>
       </c>
@@ -1550,7 +1544,7 @@
         <v>376.08</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>5</v>
       </c>
@@ -1564,7 +1558,7 @@
         <v>374.665</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>5</v>
       </c>
@@ -1578,7 +1572,7 @@
         <v>369.405</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>5</v>
       </c>
@@ -1592,7 +1586,7 @@
         <v>285.55</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>5</v>
       </c>
@@ -1606,7 +1600,7 @@
         <v>274.804</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>5</v>
       </c>
@@ -1620,7 +1614,7 @@
         <v>355.405</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>5</v>
       </c>
@@ -1634,7 +1628,7 @@
         <v>346.7</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>5</v>
       </c>
@@ -1648,7 +1642,7 @@
         <v>320.125</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>5</v>
       </c>
@@ -1662,7 +1656,7 @@
         <v>402.23</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1670,7 @@
         <v>374.435</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>5</v>
       </c>
@@ -1690,7 +1684,7 @@
         <v>334.75</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1698,7 @@
         <v>390.84</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>5</v>
       </c>
@@ -1717,12 +1711,8 @@
       <c r="D103" s="0" t="n">
         <v>382.5</v>
       </c>
-      <c r="E103" s="0" t="n">
-        <f aca="false">AVERAGE(D53:D103)</f>
-        <v>354.654411764706</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>6</v>
       </c>
@@ -1736,7 +1726,7 @@
         <v>377.3</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>6</v>
       </c>
@@ -1750,7 +1740,7 @@
         <v>321.175</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>6</v>
       </c>
@@ -1764,7 +1754,7 @@
         <v>365.64</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>6</v>
       </c>
@@ -1778,7 +1768,7 @@
         <v>334.84</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>6</v>
       </c>
@@ -1792,7 +1782,7 @@
         <v>345.78</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>6</v>
       </c>
@@ -1806,7 +1796,7 @@
         <v>326.5</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>6</v>
       </c>
@@ -1820,7 +1810,7 @@
         <v>294.17</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +1824,7 @@
         <v>343.14</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>6</v>
       </c>
@@ -1848,7 +1838,7 @@
         <v>405.986</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>6</v>
       </c>
@@ -1862,7 +1852,7 @@
         <v>387.005</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>6</v>
       </c>
@@ -1876,7 +1866,7 @@
         <v>347.415</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>6</v>
       </c>
@@ -1890,7 +1880,7 @@
         <v>377.68</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>6</v>
       </c>
@@ -1904,7 +1894,7 @@
         <v>346.436</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>6</v>
       </c>
@@ -1918,7 +1908,7 @@
         <v>366.64</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>6</v>
       </c>
@@ -1932,7 +1922,7 @@
         <v>405.65</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>6</v>
       </c>
@@ -1946,7 +1936,7 @@
         <v>369.21</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>6</v>
       </c>
@@ -1960,7 +1950,7 @@
         <v>364.48</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>6</v>
       </c>
@@ -1974,7 +1964,7 @@
         <v>311.021</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>6</v>
       </c>
@@ -1988,7 +1978,7 @@
         <v>350.85</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>6</v>
       </c>
@@ -2002,7 +1992,7 @@
         <v>358.525</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>6</v>
       </c>
@@ -2016,7 +2006,7 @@
         <v>348.79</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>6</v>
       </c>
@@ -2030,7 +2020,7 @@
         <v>340.28</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>6</v>
       </c>
@@ -2044,7 +2034,7 @@
         <v>217.5</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>6</v>
       </c>
@@ -2058,7 +2048,7 @@
         <v>340.47</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>6</v>
       </c>
@@ -2072,7 +2062,7 @@
         <v>345.425</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>6</v>
       </c>
@@ -2086,7 +2076,7 @@
         <v>391.84</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>6</v>
       </c>
@@ -2100,7 +2090,7 @@
         <v>314.05</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>6</v>
       </c>
@@ -2114,7 +2104,7 @@
         <v>330.896</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>6</v>
       </c>
@@ -2128,7 +2118,7 @@
         <v>389.36</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>6</v>
       </c>
@@ -2142,7 +2132,7 @@
         <v>377.483</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>6</v>
       </c>
@@ -2156,7 +2146,7 @@
         <v>401.276</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>6</v>
       </c>
@@ -2170,7 +2160,7 @@
         <v>408.16</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2174,7 @@
         <v>381.975</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>6</v>
       </c>
@@ -2198,7 +2188,7 @@
         <v>407.8</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>6</v>
       </c>
@@ -2212,7 +2202,7 @@
         <v>337.018</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>6</v>
       </c>
@@ -2226,7 +2216,7 @@
         <v>392.78</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>6</v>
       </c>
@@ -2240,7 +2230,7 @@
         <v>370.46</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>6</v>
       </c>
@@ -2254,7 +2244,7 @@
         <v>305.791</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>6</v>
       </c>
@@ -2268,7 +2258,7 @@
         <v>370.17</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2272,7 @@
         <v>387.81</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>6</v>
       </c>
@@ -2296,7 +2286,7 @@
         <v>380.78</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>6</v>
       </c>
@@ -2310,7 +2300,7 @@
         <v>309.9</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>6</v>
       </c>
@@ -2324,7 +2314,7 @@
         <v>375.7</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>6</v>
       </c>
@@ -2338,7 +2328,7 @@
         <v>358.87</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>6</v>
       </c>
@@ -2352,7 +2342,7 @@
         <v>390.457</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>6</v>
       </c>
@@ -2366,7 +2356,7 @@
         <v>402.27</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>6</v>
       </c>
@@ -2380,7 +2370,7 @@
         <v>365.235</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>6</v>
       </c>
@@ -2394,7 +2384,7 @@
         <v>389.09</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>6</v>
       </c>
@@ -2408,7 +2398,7 @@
         <v>404.2</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>6</v>
       </c>
@@ -2422,7 +2412,7 @@
         <v>352.525</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>6</v>
       </c>
@@ -2434,10 +2424,6 @@
       </c>
       <c r="D154" s="0" t="n">
         <v>387.5</v>
-      </c>
-      <c r="E154" s="0" t="n">
-        <f aca="false">AVERAGE(D104:D154)</f>
-        <v>360.300078431373</v>
       </c>
     </row>
   </sheetData>
@@ -2458,8 +2444,8 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2837,1424 +2823,1256 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>90.0786930969226</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>5.19268190865859</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>38.8454792104387</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>11.8387957328988</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>7.24035631645311</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>190.763647404106</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>73.0693575816694</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>2.5944762861887</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>3.67207248581626</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>8.12078133387252</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>2.9373213818731</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>77.860503479829</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>90.0786930969226</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>5.19268190865859</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>38.8454792104387</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>11.8387957328988</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>7.24035631645311</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>190.763647404106</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>73.0693575816694</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>2.5944762861887</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>3.67207248581626</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>8.12078133387252</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>2.9373213818731</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>77.860503479829</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="C3" s="0" t="n">
+        <v>91.1446020488574</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5.05724477496403</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>39.7163843857124</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>11.683511233843</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>7.69926599897688</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>172.437566321126</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>67.9169374251539</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2.54780554978379</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>3.76520127236542</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>7.78664673354878</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>2.78603382558656</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>74.6580757186878</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>89.4736842105261</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>4.88905849828593</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>39.5198895278113</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>11.8033425259788</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>7.26939835287588</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>144.230996320097</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>66.631773985429</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>2.31791133075736</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>3.33408278613513</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>7.56867840560533</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>2.74084347570508</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>69.5639893477266</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="B5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>91.3021769522673</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5.04836365144307</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>38.4913444100406</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>10.634548351186</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>4.25939289226795</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>94.4711523802136</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>73.4976650576207</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>2.12131831416018</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>4.02049344069426</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>7.45220457008244</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>2.39881983988073</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>51.1247072222932</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>90.5126928820307</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5.42081576910314</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>38.9953481698549</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>11.5406705056215</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>6.71491533500215</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>193.566318469178</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>66.6257157538622</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2.54917785534709</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>3.73744799530937</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>7.76825906062465</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>2.68855302605654</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>54.5223635940078</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>91.1446020488574</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>5.05724477496403</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>39.7163843857124</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>11.683511233843</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>7.69926599897688</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>172.437566321126</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>67.9169374251539</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>2.54780554978379</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>3.76520127236542</v>
-      </c>
-      <c r="N3" s="0" t="n">
-        <v>7.78664673354878</v>
-      </c>
-      <c r="O3" s="0" t="n">
-        <v>2.78603382558656</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>74.6580757186878</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="C7" s="0" t="n">
+        <v>91.0087719298242</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>5.20100796195949</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>39.1524330421318</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>10.1754651060049</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>5.52457017725208</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>68.905571030086</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>69.133595259329</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>2.28571187453411</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>3.73357834434547</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>8.00794238595809</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>2.58999351562284</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>47.6826367225342</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>90.8376461567952</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>4.94845101183232</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>39.0208813999776</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>12.1916649060814</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>6.41062334949956</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>150.239792931023</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>69.0746805132375</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>2.57550170527919</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>4.26677448556471</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>8.07976851524076</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>2.71421896213674</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>68.210060882098</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>90.8297809061164</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>5.03060140440116</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>39.1096926351872</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>11.8902002494975</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>9.59560337297664</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>179.186583702121</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>69.4055245271806</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>2.67761340387484</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>3.95087937240854</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>8.25700967953074</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>2.63823410130014</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>62.3053122165355</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>89.4910179640714</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>4.89183384938623</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>38.7777606435914</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>11.1072713567535</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>7.79841189553417</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>163.419275700292</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>64.5365759172309</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>2.56584120412492</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>3.18471671400031</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>8.41060662096458</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>2.7924563452583</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>59.8429979329501</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>91.1864069952309</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>4.95677706513322</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>38.9886873272142</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>11.8224464185939</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>6.38815933163753</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>137.236764267191</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>70.0817640330076</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>2.42485539984687</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>4.69117614303032</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>7.96914948618816</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>2.72526237944358</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>67.0502420619436</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>90.6186465291897</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>4.74196488997011</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>38.6190105606544</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>13.5690430150281</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>5.92555779326105</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>150.582384266848</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>70.9204372333956</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>2.49859035627268</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>4.82912526349956</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>7.6342247796801</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>2.71492106570633</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>69.6617917536868</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>90.4462413896382</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>5.05835491540414</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>38.67174223156</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>12.5860380277589</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>6.28189685647897</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>149.401624266783</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>68.5258865492276</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>2.56445148458924</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>4.80806137774359</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>8.15310129365159</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>2.85114334636954</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>67.6583458447715</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>91.9140124248093</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>4.85186879354193</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>40.2442561649892</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>10.381203697549</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>8.53348756646866</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>133.589464976074</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>66.9031534324694</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>2.26376986707582</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>4.1950668551677</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>8.2334251516616</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>2.6656761981849</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>96.5402530055257</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>90.2398105200829</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>4.66980576136235</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>39.6969569280103</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>10.3331456912503</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>6.92809671961251</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>126.629986968862</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>65.2490832436083</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>2.23753557731414</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>3.68477875516617</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>8.07098399656441</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>2.70177029466136</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>94.7869111697155</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>89.9101796407186</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>4.61596395001656</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>39.6020399203801</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>11.427617100517</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>7.41952795084187</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>139.805903672405</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>65.9690096487464</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>2.32233549441466</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>4.20997990752525</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>7.73262338003304</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>2.64301750780239</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>115.987322020272</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>89.2546823711136</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>4.88184258542516</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>39.5520836005748</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>10.3415940668709</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>7.918884905707</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>79.9131144851869</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>61.3623406067622</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>2.23105016050762</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>3.96394933834515</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>7.77164593202484</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>2.59548350671827</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>53.2568906592297</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>90.1268834258531</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>4.85852963618265</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>39.7890985845403</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>10.4525009921097</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>6.79447190120062</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>90.6038141949472</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>60.9639379538502</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>2.17854086457297</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>3.80651975651827</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>7.68332605126778</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>2.49994794612296</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>51.2930902230712</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>90.2009304167083</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>4.93013369457035</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>39.9439631759369</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>10.6607628407891</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>9.30192327696125</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>80.8542875689692</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>63.5557891782533</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>2.22601671474198</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>4.18029590813187</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>7.82456385240569</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>2.60753272217614</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>55.8541112915352</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>89.4736842105261</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>4.88905849828593</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>39.5198895278113</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>11.8033425259788</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>7.26939835287588</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>144.230996320097</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>66.631773985429</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>2.31791133075736</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>3.33408278613513</v>
-      </c>
-      <c r="N4" s="0" t="n">
-        <v>7.56867840560533</v>
-      </c>
-      <c r="O4" s="0" t="n">
-        <v>2.74084347570508</v>
-      </c>
-      <c r="P4" s="0" t="n">
-        <v>69.5639893477266</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="0" t="s">
+      <c r="B20" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>91.3429855217174</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>5.25540484352534</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>39.2817644034057</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>12.5353990395697</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>6.83469773873452</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>61.4991816391346</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>72.1606155477943</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>2.33771680224843</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>2.78452308130738</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>8.21821043173861</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>2.51016074936149</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>50.7470929966302</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>90.42365810698</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>5.12773869291161</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>38.3281537653431</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>11.8507850975801</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>4.03621991116717</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>92.9821572138414</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>72.7400577005233</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>2.36101261524624</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>2.6937324446532</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>8.44754363689515</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>2.52556387041672</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>47.8528201481182</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>90.5156078587808</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>5.17991529359722</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>38.6484292823175</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>12.4683169323498</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>4.73497325172736</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>68.3507517115603</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>69.6511196729264</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>2.3716589323918</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>2.707999696203</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>8.31151601897012</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>2.60691609940433</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>47.8558780932504</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>91.3021769522673</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>5.04836365144307</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>38.4913444100406</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>10.634548351186</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>4.25939289226795</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>94.4711523802136</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>73.4976650576207</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>2.12131831416018</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>4.02049344069426</v>
-      </c>
-      <c r="N5" s="0" t="n">
-        <v>7.45220457008244</v>
-      </c>
-      <c r="O5" s="0" t="n">
-        <v>2.39881983988073</v>
-      </c>
-      <c r="P5" s="0" t="n">
-        <v>51.1247072222932</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="C23" s="0" t="n">
+        <v>90.8311740083716</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>5.22099048988164</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>38.383105717129</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>13.5787737905821</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>6.50307944806674</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>115.232363692585</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>71.5698131019055</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>2.52962444167398</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>2.87920475231612</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>7.97715931199758</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>2.72604814669468</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>57.1639452117988</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>89.8036479617266</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>5.02394056176044</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>37.0054214309408</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>16.2822186779734</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>6.72798283469403</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>276.647900367126</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>72.527092436881</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>3.09395899411462</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>3.14035159341971</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>7.83116796085964</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>2.58234740014157</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>63.6482575205402</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>90.5126928820307</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>5.42081576910314</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>38.9953481698549</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>11.5406705056215</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>6.71491533500215</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>193.566318469178</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>66.6257157538622</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>2.54917785534709</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>3.73744799530937</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>7.76825906062465</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>2.68855302605654</v>
-      </c>
-      <c r="P6" s="0" t="n">
-        <v>54.5223635940078</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>91.0087719298242</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>5.20100796195949</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>39.1524330421318</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>10.1754651060049</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>5.52457017725208</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>68.905571030086</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>69.133595259329</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>2.28571187453411</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>3.73357834434547</v>
-      </c>
-      <c r="N7" s="0" t="n">
-        <v>8.00794238595809</v>
-      </c>
-      <c r="O7" s="0" t="n">
-        <v>2.58999351562284</v>
-      </c>
-      <c r="P7" s="0" t="n">
-        <v>47.6826367225342</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>90.8376461567952</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>4.94845101183232</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>39.0208813999776</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>12.1916649060814</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>6.41062334949956</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>150.239792931023</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>69.0746805132375</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>2.57550170527919</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>4.26677448556471</v>
-      </c>
-      <c r="N8" s="0" t="n">
-        <v>8.07976851524076</v>
-      </c>
-      <c r="O8" s="0" t="n">
-        <v>2.71421896213674</v>
-      </c>
-      <c r="P8" s="0" t="n">
-        <v>68.210060882098</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="C25" s="0" t="n">
+        <v>89.8624401913874</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>5.03060140440116</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>37.8191543735483</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>14.3105400084217</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>7.74261074188799</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>113.003985147924</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>71.4563987307616</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>2.60154734070535</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>2.80595782787402</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>8.09917522057873</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>2.57185794098003</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>59.3342473912438</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>90.2640757349277</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>4.95067129271256</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>37.3684373548599</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>14.2560542803158</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>6.89275925200135</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>141.315739621631</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>72.7987045551509</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>2.73533500121598</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>2.88275206982343</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>8.16310822439525</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>2.55905505728717</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>60.0026068184345</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>91.0210568136674</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>4.93623946699101</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>38.0511737255333</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>15.3335849533508</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>6.90011111184857</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>160.68838481542</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>75.3891294545778</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>2.83839373104811</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>2.93549768247525</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>7.89657487690135</v>
+      </c>
+      <c r="M27" s="0" t="n">
+        <v>2.63844533188043</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>59.6688088192651</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <v>90.8297809061164</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>5.03060140440116</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>39.1096926351872</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>11.8902002494975</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>9.59560337297664</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>179.186583702121</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>69.4055245271806</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>2.67761340387484</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>3.95087937240854</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>8.25700967953074</v>
-      </c>
-      <c r="O9" s="0" t="n">
-        <v>2.63823410130014</v>
-      </c>
-      <c r="P9" s="0" t="n">
-        <v>62.3053122165355</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>89.4910179640714</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>4.89183384938623</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>38.7777606435914</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>11.1072713567535</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>7.79841189553417</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>163.419275700292</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>64.5365759172309</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>2.56584120412492</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>3.18471671400031</v>
-      </c>
-      <c r="N10" s="0" t="n">
-        <v>8.41060662096458</v>
-      </c>
-      <c r="O10" s="0" t="n">
-        <v>2.7924563452583</v>
-      </c>
-      <c r="P10" s="0" t="n">
-        <v>59.8429979329501</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>91.1864069952309</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>4.95677706513322</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>38.9886873272142</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>11.8224464185939</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>6.38815933163753</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>137.236764267191</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>70.0817640330076</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>2.42485539984687</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>4.69117614303032</v>
-      </c>
-      <c r="N11" s="0" t="n">
-        <v>7.96914948618816</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <v>2.72526237944358</v>
-      </c>
-      <c r="P11" s="0" t="n">
-        <v>67.0502420619436</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>90.6186465291897</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>4.74196488997011</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>38.6190105606544</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>13.5690430150281</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>5.92555779326105</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>150.582384266848</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>70.9204372333956</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>2.49859035627268</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>4.82912526349956</v>
-      </c>
-      <c r="N12" s="0" t="n">
-        <v>7.6342247796801</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>2.71492106570633</v>
-      </c>
-      <c r="P12" s="0" t="n">
-        <v>69.6617917536868</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>90.4462413896382</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>5.05835491540414</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>38.67174223156</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>12.5860380277589</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>6.28189685647897</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>149.401624266783</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>68.5258865492276</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>2.56445148458924</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>4.80806137774359</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <v>8.15310129365159</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <v>2.85114334636954</v>
-      </c>
-      <c r="P13" s="0" t="n">
-        <v>67.6583458447715</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>91.9140124248093</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>4.85186879354193</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>40.2442561649892</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>10.381203697549</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>8.53348756646866</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>133.589464976074</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>66.9031534324694</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <v>2.26376986707582</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <v>4.1950668551677</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>8.2334251516616</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <v>2.6656761981849</v>
-      </c>
-      <c r="P14" s="0" t="n">
-        <v>96.5402530055257</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>90.2398105200829</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>4.66980576136235</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>39.6969569280103</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>10.3331456912503</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>6.92809671961251</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>126.629986968862</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>65.2490832436083</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <v>2.23753557731414</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <v>3.68477875516617</v>
-      </c>
-      <c r="N15" s="0" t="n">
-        <v>8.07098399656441</v>
-      </c>
-      <c r="O15" s="0" t="n">
-        <v>2.70177029466136</v>
-      </c>
-      <c r="P15" s="0" t="n">
-        <v>94.7869111697155</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>89.9101796407186</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>4.61596395001656</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>39.6020399203801</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>11.427617100517</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>7.41952795084187</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>139.805903672405</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>65.9690096487464</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>2.32233549441466</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>4.20997990752525</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>7.73262338003304</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <v>2.64301750780239</v>
-      </c>
-      <c r="P16" s="0" t="n">
-        <v>115.987322020272</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>89.2546823711136</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>4.88184258542516</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>39.5520836005748</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>10.3415940668709</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>7.918884905707</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>79.9131144851869</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <v>61.3623406067622</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <v>2.23105016050762</v>
-      </c>
-      <c r="M17" s="0" t="n">
-        <v>3.96394933834515</v>
-      </c>
-      <c r="N17" s="0" t="n">
-        <v>7.77164593202484</v>
-      </c>
-      <c r="O17" s="0" t="n">
-        <v>2.59548350671827</v>
-      </c>
-      <c r="P17" s="0" t="n">
-        <v>53.2568906592297</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>90.1268834258531</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>4.85852963618265</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>39.7890985845403</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>10.4525009921097</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>6.79447190120062</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>90.6038141949472</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <v>60.9639379538502</v>
-      </c>
-      <c r="L18" s="0" t="n">
-        <v>2.17854086457297</v>
-      </c>
-      <c r="M18" s="0" t="n">
-        <v>3.80651975651827</v>
-      </c>
-      <c r="N18" s="0" t="n">
-        <v>7.68332605126778</v>
-      </c>
-      <c r="O18" s="0" t="n">
-        <v>2.49994794612296</v>
-      </c>
-      <c r="P18" s="0" t="n">
-        <v>51.2930902230712</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>90.2009304167083</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>4.93013369457035</v>
-      </c>
-      <c r="G19" s="0" t="n">
-        <v>39.9439631759369</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>10.6607628407891</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>9.30192327696125</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <v>80.8542875689692</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <v>63.5557891782533</v>
-      </c>
-      <c r="L19" s="0" t="n">
-        <v>2.22601671474198</v>
-      </c>
-      <c r="M19" s="0" t="n">
-        <v>4.18029590813187</v>
-      </c>
-      <c r="N19" s="0" t="n">
-        <v>7.82456385240569</v>
-      </c>
-      <c r="O19" s="0" t="n">
-        <v>2.60753272217614</v>
-      </c>
-      <c r="P19" s="0" t="n">
-        <v>55.8541112915352</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>91.3429855217174</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>5.25540484352534</v>
-      </c>
-      <c r="G20" s="0" t="n">
-        <v>39.2817644034057</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>12.5353990395697</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>6.83469773873452</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>61.4991816391346</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <v>72.1606155477943</v>
-      </c>
-      <c r="L20" s="0" t="n">
-        <v>2.33771680224843</v>
-      </c>
-      <c r="M20" s="0" t="n">
-        <v>2.78452308130738</v>
-      </c>
-      <c r="N20" s="0" t="n">
-        <v>8.21821043173861</v>
-      </c>
-      <c r="O20" s="0" t="n">
-        <v>2.51016074936149</v>
-      </c>
-      <c r="P20" s="0" t="n">
-        <v>50.7470929966302</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>90.42365810698</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>5.12773869291161</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>38.3281537653431</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>11.8507850975801</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>4.03621991116717</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>92.9821572138414</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <v>72.7400577005233</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <v>2.36101261524624</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <v>2.6937324446532</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>8.44754363689515</v>
-      </c>
-      <c r="O21" s="0" t="n">
-        <v>2.52556387041672</v>
-      </c>
-      <c r="P21" s="0" t="n">
-        <v>47.8528201481182</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>90.5156078587808</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>5.17991529359722</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <v>38.6484292823175</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>12.4683169323498</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>4.73497325172736</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>68.3507517115603</v>
-      </c>
-      <c r="K22" s="0" t="n">
-        <v>69.6511196729264</v>
-      </c>
-      <c r="L22" s="0" t="n">
-        <v>2.3716589323918</v>
-      </c>
-      <c r="M22" s="0" t="n">
-        <v>2.707999696203</v>
-      </c>
-      <c r="N22" s="0" t="n">
-        <v>8.31151601897012</v>
-      </c>
-      <c r="O22" s="0" t="n">
-        <v>2.60691609940433</v>
-      </c>
-      <c r="P22" s="0" t="n">
-        <v>47.8558780932504</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <v>90.8311740083716</v>
-      </c>
-      <c r="F23" s="0" t="n">
-        <v>5.22099048988164</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <v>38.383105717129</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>13.5787737905821</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>6.50307944806674</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>115.232363692585</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <v>71.5698131019055</v>
-      </c>
-      <c r="L23" s="0" t="n">
-        <v>2.52962444167398</v>
-      </c>
-      <c r="M23" s="0" t="n">
-        <v>2.87920475231612</v>
-      </c>
-      <c r="N23" s="0" t="n">
-        <v>7.97715931199758</v>
-      </c>
-      <c r="O23" s="0" t="n">
-        <v>2.72604814669468</v>
-      </c>
-      <c r="P23" s="0" t="n">
-        <v>57.1639452117988</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>89.8036479617266</v>
-      </c>
-      <c r="F24" s="0" t="n">
-        <v>5.02394056176044</v>
-      </c>
-      <c r="G24" s="0" t="n">
-        <v>37.0054214309408</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <v>16.2822186779734</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>6.72798283469403</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>276.647900367126</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <v>72.527092436881</v>
-      </c>
-      <c r="L24" s="0" t="n">
-        <v>3.09395899411462</v>
-      </c>
-      <c r="M24" s="0" t="n">
-        <v>3.14035159341971</v>
-      </c>
-      <c r="N24" s="0" t="n">
-        <v>7.83116796085964</v>
-      </c>
-      <c r="O24" s="0" t="n">
-        <v>2.58234740014157</v>
-      </c>
-      <c r="P24" s="0" t="n">
-        <v>63.6482575205402</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>89.8624401913874</v>
-      </c>
-      <c r="F25" s="0" t="n">
-        <v>5.03060140440116</v>
-      </c>
-      <c r="G25" s="0" t="n">
-        <v>37.8191543735483</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>14.3105400084217</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>7.74261074188799</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>113.003985147924</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <v>71.4563987307616</v>
-      </c>
-      <c r="L25" s="0" t="n">
-        <v>2.60154734070535</v>
-      </c>
-      <c r="M25" s="0" t="n">
-        <v>2.80595782787402</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>8.09917522057873</v>
-      </c>
-      <c r="O25" s="0" t="n">
-        <v>2.57185794098003</v>
-      </c>
-      <c r="P25" s="0" t="n">
-        <v>59.3342473912438</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>90.2640757349277</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>4.95067129271256</v>
-      </c>
-      <c r="G26" s="0" t="n">
-        <v>37.3684373548599</v>
-      </c>
-      <c r="H26" s="0" t="n">
-        <v>14.2560542803158</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>6.89275925200135</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <v>141.315739621631</v>
-      </c>
-      <c r="K26" s="0" t="n">
-        <v>72.7987045551509</v>
-      </c>
-      <c r="L26" s="0" t="n">
-        <v>2.73533500121598</v>
-      </c>
-      <c r="M26" s="0" t="n">
-        <v>2.88275206982343</v>
-      </c>
-      <c r="N26" s="0" t="n">
-        <v>8.16310822439525</v>
-      </c>
-      <c r="O26" s="0" t="n">
-        <v>2.55905505728717</v>
-      </c>
-      <c r="P26" s="0" t="n">
-        <v>60.0026068184345</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>91.0210568136674</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>4.93623946699101</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <v>38.0511737255333</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>15.3335849533508</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>6.90011111184857</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>160.68838481542</v>
-      </c>
-      <c r="K27" s="0" t="n">
-        <v>75.3891294545778</v>
-      </c>
-      <c r="L27" s="0" t="n">
-        <v>2.83839373104811</v>
-      </c>
-      <c r="M27" s="0" t="n">
-        <v>2.93549768247525</v>
-      </c>
-      <c r="N27" s="0" t="n">
-        <v>7.89657487690135</v>
-      </c>
-      <c r="O27" s="0" t="n">
-        <v>2.63844533188043</v>
-      </c>
-      <c r="P27" s="0" t="n">
-        <v>59.6688088192651</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="C28" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>33</v>
+        <v>91.0172516359302</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>4.98064508459578</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>91.0172516359302</v>
+        <v>38.9415063585091</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>4.98064508459578</v>
+        <v>13.3858956197033</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>38.9415063585091</v>
+        <v>9.87912359668372</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>13.3858956197033</v>
+        <v>145.113549312496</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>9.87912359668372</v>
+        <v>67.6031781564457</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>145.113549312496</v>
+        <v>2.58231561354652</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>67.6031781564457</v>
+        <v>2.53514158373816</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>2.58231561354652</v>
+        <v>8.10843256797523</v>
       </c>
       <c r="M28" s="0" t="n">
-        <v>2.53514158373816</v>
+        <v>2.78875601996911</v>
       </c>
       <c r="N28" s="0" t="n">
-        <v>8.10843256797523</v>
-      </c>
-      <c r="O28" s="0" t="n">
-        <v>2.78875601996911</v>
-      </c>
-      <c r="P28" s="0" t="n">
         <v>59.8478638614854</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reorganization of files and folders
</commit_message>
<xml_diff>
--- a/data/lettuce.xlsx
+++ b/data/lettuce.xlsx
@@ -162,9 +162,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -232,12 +233,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -260,8 +265,8 @@
   </sheetPr>
   <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="A1:N28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E110" activeCellId="0" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2445,7 +2450,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A1:N28"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2499,31 +2504,31 @@
       <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>18761.9048407568</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>10306.0022084371</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>29067.2725</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>12684.8743733333</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>42136.9872412388</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>1504.5355</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>22010.605</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>222.039645</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>23.6618325</v>
       </c>
     </row>
@@ -2534,19 +2539,19 @@
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>21645.3542877239</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>12437.0702888756</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>34081.64285</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>11491.5018733333</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>44055.0946734834</v>
       </c>
       <c r="H3" s="1" t="n">
@@ -2558,7 +2563,7 @@
       <c r="J3" s="1" t="n">
         <v>278.241845</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>27.742095</v>
       </c>
     </row>
@@ -2569,19 +2574,19 @@
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>16838.2587876738</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>10632.1682323681</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>27469.952475</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>10355.9508733333</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>43390.3543883798</v>
       </c>
       <c r="H4" s="1" t="n">
@@ -2593,7 +2598,7 @@
       <c r="J4" s="1" t="n">
         <v>238.926895</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>19.1389333333333</v>
       </c>
     </row>
@@ -2604,31 +2609,31 @@
       <c r="B5" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>20802.8090137028</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>11967.7068383223</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>31895.044325</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>12630.3224418333</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>41029.9961148252</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>1439.81973474096</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>26337.7301089178</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="1" t="n">
         <v>335.542441960721</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>28.9492125</v>
       </c>
     </row>
@@ -2639,31 +2644,31 @@
       <c r="B6" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>21772.6966289723</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>11997.3568460277</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>33770.053475</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>10672.2162862551</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>47175.575985864</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>1467.01863862725</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <v>21585.5732755892</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
         <v>316.188489629775</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>29.377145</v>
       </c>
     </row>
@@ -2674,31 +2679,31 @@
       <c r="B7" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>17620.2957964464</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>13936.7169285536</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>31557.012725</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>11265.6729174381</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>42896.9508468937</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>1502.48748702529</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>24398.428146034</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="1" t="n">
         <v>257.110626416756</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>25.0036639005855</v>
       </c>
     </row>
@@ -2709,31 +2714,31 @@
       <c r="B8" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>20342.6542214464</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>13938.8424285536</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>34281.49665</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>9118.48575704411</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>47207.9978827914</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>1394.8993926275</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <v>19296.3288426945</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="1" t="n">
         <v>285.840136360119</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>31.025050041332</v>
       </c>
     </row>
@@ -2744,31 +2749,31 @@
       <c r="B9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>21635.1065713069</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>15013.8777023229</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>36648.9842736298</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>6988.36075703265</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>46268.123501614</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>1730.13032705656</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <v>15865.5454860459</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="1" t="n">
         <v>265.159355</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>29.7709824206659</v>
       </c>
     </row>
@@ -2779,31 +2784,31 @@
       <c r="B10" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>22563.0404511268</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>12648.0089488732</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>35211.0494</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>10432.1434292257</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>40841.1318303571</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>1348.28810098257</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <v>22660.4840070055</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="1" t="n">
         <v>301.044988289245</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>25.8682772079741</v>
       </c>
     </row>
@@ -2826,7 +2831,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:N28"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2885,40 +2890,40 @@
       <c r="B2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>90.0786930969226</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>5.19268190865859</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="2" t="n">
         <v>38.8454792104387</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>11.8387957328988</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="2" t="n">
         <v>7.24035631645311</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="2" t="n">
         <v>190.763647404106</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="2" t="n">
         <v>73.0693575816694</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="2" t="n">
         <v>2.5944762861887</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="2" t="n">
         <v>3.67207248581626</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="2" t="n">
         <v>8.12078133387252</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="2" t="n">
         <v>2.9373213818731</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="2" t="n">
         <v>77.860503479829</v>
       </c>
     </row>
@@ -2929,40 +2934,40 @@
       <c r="B3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>91.1446020488574</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>5.05724477496403</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="2" t="n">
         <v>39.7163843857124</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>11.683511233843</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="2" t="n">
         <v>7.69926599897688</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="2" t="n">
         <v>172.437566321126</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="2" t="n">
         <v>67.9169374251539</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="2" t="n">
         <v>2.54780554978379</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="2" t="n">
         <v>3.76520127236542</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="2" t="n">
         <v>7.78664673354878</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="2" t="n">
         <v>2.78603382558656</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="2" t="n">
         <v>74.6580757186878</v>
       </c>
     </row>
@@ -2973,40 +2978,40 @@
       <c r="B4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="2" t="n">
         <v>89.4736842105261</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <v>4.88905849828593</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
         <v>39.5198895278113</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
         <v>11.8033425259788</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="2" t="n">
         <v>7.26939835287588</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="2" t="n">
         <v>144.230996320097</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="2" t="n">
         <v>66.631773985429</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="2" t="n">
         <v>2.31791133075736</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="2" t="n">
         <v>3.33408278613513</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="2" t="n">
         <v>7.56867840560533</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="2" t="n">
         <v>2.74084347570508</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="2" t="n">
         <v>69.5639893477266</v>
       </c>
     </row>
@@ -3017,40 +3022,40 @@
       <c r="B5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="2" t="n">
         <v>91.3021769522673</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
         <v>5.04836365144307</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="2" t="n">
         <v>38.4913444100406</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
         <v>10.634548351186</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="2" t="n">
         <v>4.25939289226795</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="2" t="n">
         <v>94.4711523802136</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="2" t="n">
         <v>73.4976650576207</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="2" t="n">
         <v>2.12131831416018</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="2" t="n">
         <v>4.02049344069426</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="2" t="n">
         <v>7.45220457008244</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="2" t="n">
         <v>2.39881983988073</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="2" t="n">
         <v>51.1247072222932</v>
       </c>
     </row>
@@ -3061,40 +3066,40 @@
       <c r="B6" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="2" t="n">
         <v>90.5126928820307</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="2" t="n">
         <v>5.42081576910314</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="2" t="n">
         <v>38.9953481698549</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <v>11.5406705056215</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="2" t="n">
         <v>6.71491533500215</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="2" t="n">
         <v>193.566318469178</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="2" t="n">
         <v>66.6257157538622</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="2" t="n">
         <v>2.54917785534709</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="2" t="n">
         <v>3.73744799530937</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="2" t="n">
         <v>7.76825906062465</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="2" t="n">
         <v>2.68855302605654</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="2" t="n">
         <v>54.5223635940078</v>
       </c>
     </row>
@@ -3105,40 +3110,40 @@
       <c r="B7" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="2" t="n">
         <v>91.0087719298242</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2" t="n">
         <v>5.20100796195949</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="2" t="n">
         <v>39.1524330421318</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="n">
         <v>10.1754651060049</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="2" t="n">
         <v>5.52457017725208</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="2" t="n">
         <v>68.905571030086</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="2" t="n">
         <v>69.133595259329</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="2" t="n">
         <v>2.28571187453411</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="2" t="n">
         <v>3.73357834434547</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="2" t="n">
         <v>8.00794238595809</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="2" t="n">
         <v>2.58999351562284</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="2" t="n">
         <v>47.6826367225342</v>
       </c>
     </row>
@@ -3149,40 +3154,40 @@
       <c r="B8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <v>90.8376461567952</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="2" t="n">
         <v>4.94845101183232</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="2" t="n">
         <v>39.0208813999776</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
         <v>12.1916649060814</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="2" t="n">
         <v>6.41062334949956</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="2" t="n">
         <v>150.239792931023</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="2" t="n">
         <v>69.0746805132375</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="2" t="n">
         <v>2.57550170527919</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="2" t="n">
         <v>4.26677448556471</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="2" t="n">
         <v>8.07976851524076</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="2" t="n">
         <v>2.71421896213674</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="2" t="n">
         <v>68.210060882098</v>
       </c>
     </row>
@@ -3193,40 +3198,40 @@
       <c r="B9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="2" t="n">
         <v>90.8297809061164</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2" t="n">
         <v>5.03060140440116</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="2" t="n">
         <v>39.1096926351872</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <v>11.8902002494975</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="2" t="n">
         <v>9.59560337297664</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="2" t="n">
         <v>179.186583702121</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="2" t="n">
         <v>69.4055245271806</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="2" t="n">
         <v>2.67761340387484</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="2" t="n">
         <v>3.95087937240854</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="2" t="n">
         <v>8.25700967953074</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="2" t="n">
         <v>2.63823410130014</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="2" t="n">
         <v>62.3053122165355</v>
       </c>
     </row>
@@ -3237,40 +3242,40 @@
       <c r="B10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="2" t="n">
         <v>89.4910179640714</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="2" t="n">
         <v>4.89183384938623</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="2" t="n">
         <v>38.7777606435914</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <v>11.1072713567535</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="2" t="n">
         <v>7.79841189553417</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="2" t="n">
         <v>163.419275700292</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="2" t="n">
         <v>64.5365759172309</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="2" t="n">
         <v>2.56584120412492</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="2" t="n">
         <v>3.18471671400031</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="2" t="n">
         <v>8.41060662096458</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="2" t="n">
         <v>2.7924563452583</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="2" t="n">
         <v>59.8429979329501</v>
       </c>
     </row>
@@ -3281,40 +3286,40 @@
       <c r="B11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="2" t="n">
         <v>91.1864069952309</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="2" t="n">
         <v>4.95677706513322</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="2" t="n">
         <v>38.9886873272142</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="2" t="n">
         <v>11.8224464185939</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="2" t="n">
         <v>6.38815933163753</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="2" t="n">
         <v>137.236764267191</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11" s="2" t="n">
         <v>70.0817640330076</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="2" t="n">
         <v>2.42485539984687</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11" s="2" t="n">
         <v>4.69117614303032</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11" s="2" t="n">
         <v>7.96914948618816</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M11" s="2" t="n">
         <v>2.72526237944358</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N11" s="2" t="n">
         <v>67.0502420619436</v>
       </c>
     </row>
@@ -3325,40 +3330,40 @@
       <c r="B12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="2" t="n">
         <v>90.6186465291897</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="2" t="n">
         <v>4.74196488997011</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="2" t="n">
         <v>38.6190105606544</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="2" t="n">
         <v>13.5690430150281</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="2" t="n">
         <v>5.92555779326105</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="2" t="n">
         <v>150.582384266848</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12" s="2" t="n">
         <v>70.9204372333956</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="2" t="n">
         <v>2.49859035627268</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12" s="2" t="n">
         <v>4.82912526349956</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L12" s="2" t="n">
         <v>7.6342247796801</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="2" t="n">
         <v>2.71492106570633</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N12" s="2" t="n">
         <v>69.6617917536868</v>
       </c>
     </row>
@@ -3369,40 +3374,40 @@
       <c r="B13" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="2" t="n">
         <v>90.4462413896382</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="2" t="n">
         <v>5.05835491540414</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="2" t="n">
         <v>38.67174223156</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="2" t="n">
         <v>12.5860380277589</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="2" t="n">
         <v>6.28189685647897</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="2" t="n">
         <v>149.401624266783</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I13" s="2" t="n">
         <v>68.5258865492276</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="2" t="n">
         <v>2.56445148458924</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K13" s="2" t="n">
         <v>4.80806137774359</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L13" s="2" t="n">
         <v>8.15310129365159</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M13" s="2" t="n">
         <v>2.85114334636954</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N13" s="2" t="n">
         <v>67.6583458447715</v>
       </c>
     </row>
@@ -3413,40 +3418,40 @@
       <c r="B14" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="2" t="n">
         <v>91.9140124248093</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="2" t="n">
         <v>4.85186879354193</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="2" t="n">
         <v>40.2442561649892</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="2" t="n">
         <v>10.381203697549</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="2" t="n">
         <v>8.53348756646866</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="2" t="n">
         <v>133.589464976074</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="I14" s="2" t="n">
         <v>66.9031534324694</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="2" t="n">
         <v>2.26376986707582</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="K14" s="2" t="n">
         <v>4.1950668551677</v>
       </c>
-      <c r="L14" s="0" t="n">
+      <c r="L14" s="2" t="n">
         <v>8.2334251516616</v>
       </c>
-      <c r="M14" s="0" t="n">
+      <c r="M14" s="2" t="n">
         <v>2.6656761981849</v>
       </c>
-      <c r="N14" s="0" t="n">
+      <c r="N14" s="2" t="n">
         <v>96.5402530055257</v>
       </c>
     </row>
@@ -3457,40 +3462,40 @@
       <c r="B15" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="2" t="n">
         <v>90.2398105200829</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="2" t="n">
         <v>4.66980576136235</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="2" t="n">
         <v>39.6969569280103</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="2" t="n">
         <v>10.3331456912503</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="2" t="n">
         <v>6.92809671961251</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="2" t="n">
         <v>126.629986968862</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="2" t="n">
         <v>65.2490832436083</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="2" t="n">
         <v>2.23753557731414</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="2" t="n">
         <v>3.68477875516617</v>
       </c>
-      <c r="L15" s="0" t="n">
+      <c r="L15" s="2" t="n">
         <v>8.07098399656441</v>
       </c>
-      <c r="M15" s="0" t="n">
+      <c r="M15" s="2" t="n">
         <v>2.70177029466136</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="N15" s="2" t="n">
         <v>94.7869111697155</v>
       </c>
     </row>
@@ -3501,40 +3506,40 @@
       <c r="B16" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="2" t="n">
         <v>89.9101796407186</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="2" t="n">
         <v>4.61596395001656</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="2" t="n">
         <v>39.6020399203801</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="2" t="n">
         <v>11.427617100517</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="2" t="n">
         <v>7.41952795084187</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="2" t="n">
         <v>139.805903672405</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="I16" s="2" t="n">
         <v>65.9690096487464</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="2" t="n">
         <v>2.32233549441466</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="K16" s="2" t="n">
         <v>4.20997990752525</v>
       </c>
-      <c r="L16" s="0" t="n">
+      <c r="L16" s="2" t="n">
         <v>7.73262338003304</v>
       </c>
-      <c r="M16" s="0" t="n">
+      <c r="M16" s="2" t="n">
         <v>2.64301750780239</v>
       </c>
-      <c r="N16" s="0" t="n">
+      <c r="N16" s="2" t="n">
         <v>115.987322020272</v>
       </c>
     </row>
@@ -3545,40 +3550,40 @@
       <c r="B17" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="2" t="n">
         <v>89.2546823711136</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="2" t="n">
         <v>4.88184258542516</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="2" t="n">
         <v>39.5520836005748</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="2" t="n">
         <v>10.3415940668709</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="2" t="n">
         <v>7.918884905707</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="2" t="n">
         <v>79.9131144851869</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="I17" s="2" t="n">
         <v>61.3623406067622</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="2" t="n">
         <v>2.23105016050762</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="K17" s="2" t="n">
         <v>3.96394933834515</v>
       </c>
-      <c r="L17" s="0" t="n">
+      <c r="L17" s="2" t="n">
         <v>7.77164593202484</v>
       </c>
-      <c r="M17" s="0" t="n">
+      <c r="M17" s="2" t="n">
         <v>2.59548350671827</v>
       </c>
-      <c r="N17" s="0" t="n">
+      <c r="N17" s="2" t="n">
         <v>53.2568906592297</v>
       </c>
     </row>
@@ -3589,40 +3594,40 @@
       <c r="B18" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="2" t="n">
         <v>90.1268834258531</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="2" t="n">
         <v>4.85852963618265</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="2" t="n">
         <v>39.7890985845403</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="2" t="n">
         <v>10.4525009921097</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="2" t="n">
         <v>6.79447190120062</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="2" t="n">
         <v>90.6038141949472</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="I18" s="2" t="n">
         <v>60.9639379538502</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="2" t="n">
         <v>2.17854086457297</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="K18" s="2" t="n">
         <v>3.80651975651827</v>
       </c>
-      <c r="L18" s="0" t="n">
+      <c r="L18" s="2" t="n">
         <v>7.68332605126778</v>
       </c>
-      <c r="M18" s="0" t="n">
+      <c r="M18" s="2" t="n">
         <v>2.49994794612296</v>
       </c>
-      <c r="N18" s="0" t="n">
+      <c r="N18" s="2" t="n">
         <v>51.2930902230712</v>
       </c>
     </row>
@@ -3633,40 +3638,40 @@
       <c r="B19" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="2" t="n">
         <v>90.2009304167083</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="2" t="n">
         <v>4.93013369457035</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="2" t="n">
         <v>39.9439631759369</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="2" t="n">
         <v>10.6607628407891</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="2" t="n">
         <v>9.30192327696125</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="2" t="n">
         <v>80.8542875689692</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="I19" s="2" t="n">
         <v>63.5557891782533</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="2" t="n">
         <v>2.22601671474198</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="K19" s="2" t="n">
         <v>4.18029590813187</v>
       </c>
-      <c r="L19" s="0" t="n">
+      <c r="L19" s="2" t="n">
         <v>7.82456385240569</v>
       </c>
-      <c r="M19" s="0" t="n">
+      <c r="M19" s="2" t="n">
         <v>2.60753272217614</v>
       </c>
-      <c r="N19" s="0" t="n">
+      <c r="N19" s="2" t="n">
         <v>55.8541112915352</v>
       </c>
     </row>
@@ -3677,40 +3682,40 @@
       <c r="B20" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="2" t="n">
         <v>91.3429855217174</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="2" t="n">
         <v>5.25540484352534</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="2" t="n">
         <v>39.2817644034057</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="2" t="n">
         <v>12.5353990395697</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="2" t="n">
         <v>6.83469773873452</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="2" t="n">
         <v>61.4991816391346</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="I20" s="2" t="n">
         <v>72.1606155477943</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="2" t="n">
         <v>2.33771680224843</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="K20" s="2" t="n">
         <v>2.78452308130738</v>
       </c>
-      <c r="L20" s="0" t="n">
+      <c r="L20" s="2" t="n">
         <v>8.21821043173861</v>
       </c>
-      <c r="M20" s="0" t="n">
+      <c r="M20" s="2" t="n">
         <v>2.51016074936149</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="2" t="n">
         <v>50.7470929966302</v>
       </c>
     </row>
@@ -3721,40 +3726,40 @@
       <c r="B21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="2" t="n">
         <v>90.42365810698</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="2" t="n">
         <v>5.12773869291161</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="2" t="n">
         <v>38.3281537653431</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="2" t="n">
         <v>11.8507850975801</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="2" t="n">
         <v>4.03621991116717</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="2" t="n">
         <v>92.9821572138414</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="I21" s="2" t="n">
         <v>72.7400577005233</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21" s="2" t="n">
         <v>2.36101261524624</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="K21" s="2" t="n">
         <v>2.6937324446532</v>
       </c>
-      <c r="L21" s="0" t="n">
+      <c r="L21" s="2" t="n">
         <v>8.44754363689515</v>
       </c>
-      <c r="M21" s="0" t="n">
+      <c r="M21" s="2" t="n">
         <v>2.52556387041672</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="N21" s="2" t="n">
         <v>47.8528201481182</v>
       </c>
     </row>
@@ -3765,40 +3770,40 @@
       <c r="B22" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="2" t="n">
         <v>90.5156078587808</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="2" t="n">
         <v>5.17991529359722</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="2" t="n">
         <v>38.6484292823175</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="2" t="n">
         <v>12.4683169323498</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="2" t="n">
         <v>4.73497325172736</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="2" t="n">
         <v>68.3507517115603</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="2" t="n">
         <v>69.6511196729264</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="2" t="n">
         <v>2.3716589323918</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="K22" s="2" t="n">
         <v>2.707999696203</v>
       </c>
-      <c r="L22" s="0" t="n">
+      <c r="L22" s="2" t="n">
         <v>8.31151601897012</v>
       </c>
-      <c r="M22" s="0" t="n">
+      <c r="M22" s="2" t="n">
         <v>2.60691609940433</v>
       </c>
-      <c r="N22" s="0" t="n">
+      <c r="N22" s="2" t="n">
         <v>47.8558780932504</v>
       </c>
     </row>
@@ -3809,40 +3814,40 @@
       <c r="B23" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="2" t="n">
         <v>90.8311740083716</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="2" t="n">
         <v>5.22099048988164</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="2" t="n">
         <v>38.383105717129</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="2" t="n">
         <v>13.5787737905821</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="2" t="n">
         <v>6.50307944806674</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="2" t="n">
         <v>115.232363692585</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="I23" s="2" t="n">
         <v>71.5698131019055</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="J23" s="2" t="n">
         <v>2.52962444167398</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="K23" s="2" t="n">
         <v>2.87920475231612</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="L23" s="2" t="n">
         <v>7.97715931199758</v>
       </c>
-      <c r="M23" s="0" t="n">
+      <c r="M23" s="2" t="n">
         <v>2.72604814669468</v>
       </c>
-      <c r="N23" s="0" t="n">
+      <c r="N23" s="2" t="n">
         <v>57.1639452117988</v>
       </c>
     </row>
@@ -3853,40 +3858,40 @@
       <c r="B24" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="2" t="n">
         <v>89.8036479617266</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="2" t="n">
         <v>5.02394056176044</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="2" t="n">
         <v>37.0054214309408</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="2" t="n">
         <v>16.2822186779734</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="2" t="n">
         <v>6.72798283469403</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="2" t="n">
         <v>276.647900367126</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="I24" s="2" t="n">
         <v>72.527092436881</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="J24" s="2" t="n">
         <v>3.09395899411462</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="K24" s="2" t="n">
         <v>3.14035159341971</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="L24" s="2" t="n">
         <v>7.83116796085964</v>
       </c>
-      <c r="M24" s="0" t="n">
+      <c r="M24" s="2" t="n">
         <v>2.58234740014157</v>
       </c>
-      <c r="N24" s="0" t="n">
+      <c r="N24" s="2" t="n">
         <v>63.6482575205402</v>
       </c>
     </row>
@@ -3897,40 +3902,40 @@
       <c r="B25" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="2" t="n">
         <v>89.8624401913874</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="2" t="n">
         <v>5.03060140440116</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="2" t="n">
         <v>37.8191543735483</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="2" t="n">
         <v>14.3105400084217</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="2" t="n">
         <v>7.74261074188799</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="2" t="n">
         <v>113.003985147924</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="I25" s="2" t="n">
         <v>71.4563987307616</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="J25" s="2" t="n">
         <v>2.60154734070535</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="K25" s="2" t="n">
         <v>2.80595782787402</v>
       </c>
-      <c r="L25" s="0" t="n">
+      <c r="L25" s="2" t="n">
         <v>8.09917522057873</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="M25" s="2" t="n">
         <v>2.57185794098003</v>
       </c>
-      <c r="N25" s="0" t="n">
+      <c r="N25" s="2" t="n">
         <v>59.3342473912438</v>
       </c>
     </row>
@@ -3941,40 +3946,40 @@
       <c r="B26" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="2" t="n">
         <v>90.2640757349277</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="2" t="n">
         <v>4.95067129271256</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="2" t="n">
         <v>37.3684373548599</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="2" t="n">
         <v>14.2560542803158</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="2" t="n">
         <v>6.89275925200135</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="2" t="n">
         <v>141.315739621631</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="2" t="n">
         <v>72.7987045551509</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="J26" s="2" t="n">
         <v>2.73533500121598</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K26" s="2" t="n">
         <v>2.88275206982343</v>
       </c>
-      <c r="L26" s="0" t="n">
+      <c r="L26" s="2" t="n">
         <v>8.16310822439525</v>
       </c>
-      <c r="M26" s="0" t="n">
+      <c r="M26" s="2" t="n">
         <v>2.55905505728717</v>
       </c>
-      <c r="N26" s="0" t="n">
+      <c r="N26" s="2" t="n">
         <v>60.0026068184345</v>
       </c>
     </row>
@@ -3985,40 +3990,40 @@
       <c r="B27" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="2" t="n">
         <v>91.0210568136674</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="2" t="n">
         <v>4.93623946699101</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="2" t="n">
         <v>38.0511737255333</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="2" t="n">
         <v>15.3335849533508</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="2" t="n">
         <v>6.90011111184857</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="2" t="n">
         <v>160.68838481542</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="I27" s="2" t="n">
         <v>75.3891294545778</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="J27" s="2" t="n">
         <v>2.83839373104811</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="K27" s="2" t="n">
         <v>2.93549768247525</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="L27" s="2" t="n">
         <v>7.89657487690135</v>
       </c>
-      <c r="M27" s="0" t="n">
+      <c r="M27" s="2" t="n">
         <v>2.63844533188043</v>
       </c>
-      <c r="N27" s="0" t="n">
+      <c r="N27" s="2" t="n">
         <v>59.6688088192651</v>
       </c>
     </row>
@@ -4029,40 +4034,40 @@
       <c r="B28" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="2" t="n">
         <v>91.0172516359302</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="2" t="n">
         <v>4.98064508459578</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="2" t="n">
         <v>38.9415063585091</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="2" t="n">
         <v>13.3858956197033</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="2" t="n">
         <v>9.87912359668372</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="2" t="n">
         <v>145.113549312496</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="I28" s="2" t="n">
         <v>67.6031781564457</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="J28" s="2" t="n">
         <v>2.58231561354652</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="K28" s="2" t="n">
         <v>2.53514158373816</v>
       </c>
-      <c r="L28" s="0" t="n">
+      <c r="L28" s="2" t="n">
         <v>8.10843256797523</v>
       </c>
-      <c r="M28" s="0" t="n">
+      <c r="M28" s="2" t="n">
         <v>2.78875601996911</v>
       </c>
-      <c r="N28" s="0" t="n">
+      <c r="N28" s="2" t="n">
         <v>59.8478638614854</v>
       </c>
     </row>

</xml_diff>